<commit_message>
Fix result, add tests
</commit_message>
<xml_diff>
--- a/Excel_Data/2.xlsx
+++ b/Excel_Data/2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18324" windowHeight="9372"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18324" windowHeight="9372" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="5" r:id="rId1"/>
@@ -226,64 +226,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.89159839299999999</c:v>
+                  <c:v>1.9047595879999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88649849000000003</c:v>
+                  <c:v>1.6372711600000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.78476864599999996</c:v>
+                  <c:v>1.443286721</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.71030030700000002</c:v>
+                  <c:v>1.3056021710000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66031703399999997</c:v>
+                  <c:v>1.2100407959999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.62660321699999999</c:v>
+                  <c:v>1.1438732410000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60356510100000005</c:v>
+                  <c:v>1.0978559349999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58764697899999996</c:v>
+                  <c:v>1.0656603090000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.57654287900000001</c:v>
+                  <c:v>1.042995737</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.56872575199999997</c:v>
+                  <c:v>1.0269441479999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.56319391699999999</c:v>
+                  <c:v>1.0155089150000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.55923497200000005</c:v>
+                  <c:v>1.00731533</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.55639856399999998</c:v>
+                  <c:v>1.001411246</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.55434677200000004</c:v>
+                  <c:v>0.99713343600000004</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.55285921000000005</c:v>
+                  <c:v>0.99401735400000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.55177585600000001</c:v>
+                  <c:v>0.99173581799999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.55097579600000002</c:v>
+                  <c:v>0.99005711299999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.55039095699999996</c:v>
+                  <c:v>0.98881622199999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.549955207</c:v>
+                  <c:v>0.98789496899999996</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.54963043499999997</c:v>
+                  <c:v>0.98720825499999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -392,64 +392,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.84578794700000004</c:v>
+                  <c:v>2.2202717750000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97297827100000001</c:v>
+                  <c:v>1.906407704</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.92492790899999999</c:v>
+                  <c:v>1.743074867</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.88369139100000005</c:v>
+                  <c:v>1.647882598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86093504899999995</c:v>
+                  <c:v>1.5957947370000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84941587900000004</c:v>
+                  <c:v>1.568624631</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.84370419799999996</c:v>
+                  <c:v>1.554790557</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.84088365099999995</c:v>
+                  <c:v>1.5478123669999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.83947799499999998</c:v>
+                  <c:v>1.544294209</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.83876762500000002</c:v>
+                  <c:v>1.5425119169999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.83841194799999996</c:v>
+                  <c:v>1.541601722</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.838229106</c:v>
+                  <c:v>1.54113225</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.83814010400000005</c:v>
+                  <c:v>1.5408874299999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.83809098900000001</c:v>
+                  <c:v>1.5407583060000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.83807003999999996</c:v>
+                  <c:v>1.540689435</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.83805931300000003</c:v>
+                  <c:v>1.540652304</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.83805546600000003</c:v>
+                  <c:v>1.5406320849999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.83805228799999998</c:v>
+                  <c:v>1.5406209740000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.83805280800000004</c:v>
+                  <c:v>1.540614819</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.83805343700000001</c:v>
+                  <c:v>1.540611384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -558,64 +558,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.98670907799999996</c:v>
+                  <c:v>2.657843765</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80652002899999997</c:v>
+                  <c:v>2.2476537969999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64205165799999997</c:v>
+                  <c:v>2.1074637389999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70602313999999999</c:v>
+                  <c:v>2.0463224719999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78627315600000003</c:v>
+                  <c:v>2.0196704259999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82873205400000005</c:v>
+                  <c:v>2.008500937</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.85049989800000003</c:v>
+                  <c:v>2.0039550290000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86085452500000004</c:v>
+                  <c:v>2.0021353679999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.860258525</c:v>
+                  <c:v>2.0014121490000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.85933168999999998</c:v>
+                  <c:v>2.0011248269999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.85985331799999998</c:v>
+                  <c:v>2.0010101950000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.86006689300000005</c:v>
+                  <c:v>2.0009641249999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.86015311500000002</c:v>
+                  <c:v>2.0009454400000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.86018769500000003</c:v>
+                  <c:v>2.0009377879999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.86020150299999998</c:v>
+                  <c:v>2.000934623</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.86020701099999997</c:v>
+                  <c:v>2.0009333030000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.86020920000000001</c:v>
+                  <c:v>2.0009327469999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.86021006499999997</c:v>
+                  <c:v>2.000932513</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.860009001</c:v>
+                  <c:v>2.0009324130000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.86000913300000004</c:v>
+                  <c:v>2.0009323700000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -724,64 +724,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.37887468</c:v>
+                  <c:v>3.2033417790000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3811905179999999</c:v>
+                  <c:v>2.6667503739999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.204372706</c:v>
+                  <c:v>2.524938938</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.440764081</c:v>
+                  <c:v>2.4776554640000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.844072224</c:v>
+                  <c:v>2.4614160730000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2140574040000001</c:v>
+                  <c:v>2.4555925510000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5082710459999999</c:v>
+                  <c:v>2.4534809989999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.732456209</c:v>
+                  <c:v>2.452707856</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8882100909999999</c:v>
+                  <c:v>2.4524213750000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.005277446</c:v>
+                  <c:v>2.452313642</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0821550680000001</c:v>
+                  <c:v>2.4522724220000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1349551029999998</c:v>
+                  <c:v>2.4522563540000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1725827290000002</c:v>
+                  <c:v>2.4522499720000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.196329843</c:v>
+                  <c:v>2.4522473910000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2082232180000001</c:v>
+                  <c:v>2.4522463299999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2135334109999998</c:v>
+                  <c:v>2.4522458889999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2201323629999998</c:v>
+                  <c:v>2.452245703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2247391080000001</c:v>
+                  <c:v>2.4522456240000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.2278067240000001</c:v>
+                  <c:v>2.45224559</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.2297245440000002</c:v>
+                  <c:v>2.4522455760000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,11 +797,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-268916304"/>
-        <c:axId val="-268909776"/>
+        <c:axId val="1970021488"/>
+        <c:axId val="1970024752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-268916304"/>
+        <c:axId val="1970021488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -844,7 +844,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-268909776"/>
+        <c:crossAx val="1970024752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -852,7 +852,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-268909776"/>
+        <c:axId val="1970024752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -903,7 +903,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-268916304"/>
+        <c:crossAx val="1970021488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1037,64 +1037,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.12860655100000001</c:v>
+                  <c:v>0.16728716599999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.0159904000000003E-2</c:v>
+                  <c:v>0.34014248000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.0761482E-2</c:v>
+                  <c:v>0.58845096799999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.2080589E-2</c:v>
+                  <c:v>0.887835441</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2148706999999999E-2</c:v>
+                  <c:v>1.209767939</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2215292E-2</c:v>
+                  <c:v>1.535671896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.221537E-2</c:v>
+                  <c:v>1.854602343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>2.1605089030000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>2.4504152719999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>2.7232547820000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>2.9791196590000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>3.218774233</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>3.4433406030000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>3.6540984380000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>3.8523605839999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>4.0393987989999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2215375999999997E-2</c:v>
+                  <c:v>4.2164022719999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2215343E-2</c:v>
+                  <c:v>4.384457287</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.2215343E-2</c:v>
+                  <c:v>4.5445401710000004</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.2215343E-2</c:v>
+                  <c:v>4.6975183530000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1134,64 +1134,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.50616134999999995</c:v>
+                  <c:v>0.29893379199999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.29139865700000001</c:v>
+                  <c:v>0.51668483799999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.22048114799999999</c:v>
+                  <c:v>0.74617820000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.229747388</c:v>
+                  <c:v>0.98713218300000005</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23700928900000001</c:v>
+                  <c:v>1.216379541</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.23909171700000001</c:v>
+                  <c:v>1.4212518590000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23905536499999999</c:v>
+                  <c:v>1.5989392499999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.239102747</c:v>
+                  <c:v>1.7513704590000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.23911279999999999</c:v>
+                  <c:v>1.8820732120000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23911487100000001</c:v>
+                  <c:v>1.9947453639999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.239115296</c:v>
+                  <c:v>2.0927140569999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.23911538299999999</c:v>
+                  <c:v>2.178787942</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.23911540000000001</c:v>
+                  <c:v>2.2552662379999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.23910288299999999</c:v>
+                  <c:v>2.3240015380000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.23910288299999999</c:v>
+                  <c:v>2.3864740229999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.23910288399999999</c:v>
+                  <c:v>2.443860999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.23910288399999999</c:v>
+                  <c:v>2.497096703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23910288399999999</c:v>
+                  <c:v>2.5469217209999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.23910288399999999</c:v>
+                  <c:v>2.5939230100000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.23910288399999999</c:v>
+                  <c:v>2.6385659330000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1231,64 +1231,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.98670907799999996</c:v>
+                  <c:v>0.40426259599999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80652002899999997</c:v>
+                  <c:v>0.69034385600000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64205165799999997</c:v>
+                  <c:v>0.92072630899999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.70602313999999999</c:v>
+                  <c:v>1.118072161</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.78627315600000003</c:v>
+                  <c:v>1.2833249790000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.82873205400000005</c:v>
+                  <c:v>1.418161303</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.85049989800000003</c:v>
+                  <c:v>1.5271453989999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86085452500000004</c:v>
+                  <c:v>1.615515313</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.860258525</c:v>
+                  <c:v>1.6879366499999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.85933168999999998</c:v>
+                  <c:v>1.7481742069999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.85985331799999998</c:v>
+                  <c:v>1.7991414450000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.86006689300000005</c:v>
+                  <c:v>1.843052403</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.86015311500000002</c:v>
+                  <c:v>1.88157643</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.86018769500000003</c:v>
+                  <c:v>1.9159680690000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.86020150299999998</c:v>
+                  <c:v>1.9471690239999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.86020701099999997</c:v>
+                  <c:v>1.975886056</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.86020920000000001</c:v>
+                  <c:v>2.0026498290000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.86021006499999997</c:v>
+                  <c:v>2.0278591129999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.860009001</c:v>
+                  <c:v>2.0518139340000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.86000913300000004</c:v>
+                  <c:v>2.0747403879999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,64 +1328,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.37887468</c:v>
+                  <c:v>0.49034151999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3811905179999999</c:v>
+                  <c:v>0.86019787400000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.204372706</c:v>
+                  <c:v>1.1304277899999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.440764081</c:v>
+                  <c:v>1.3266246399999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.844072224</c:v>
+                  <c:v>1.4702520640000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2140574040000001</c:v>
+                  <c:v>1.577077214</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.5082710459999999</c:v>
+                  <c:v>1.6580968410000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.732456209</c:v>
+                  <c:v>1.720868646</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.8882100909999999</c:v>
+                  <c:v>1.7706135119999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.005277446</c:v>
+                  <c:v>1.8109810289999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.0821550680000001</c:v>
+                  <c:v>1.84455076</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.1349551029999998</c:v>
+                  <c:v>1.8731605419999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.1725827290000002</c:v>
+                  <c:v>1.898126457</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.196329843</c:v>
+                  <c:v>1.9203939569999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2082232180000001</c:v>
+                  <c:v>1.9406436460000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.2135334109999998</c:v>
+                  <c:v>1.959366242</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.2201323629999998</c:v>
+                  <c:v>1.9769160539999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.2247391080000001</c:v>
+                  <c:v>1.9935493129999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.2278067240000001</c:v>
+                  <c:v>2.0094516809999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.2297245440000002</c:v>
+                  <c:v>2.024758024</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,11 +1401,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-516952208"/>
-        <c:axId val="-516951664"/>
+        <c:axId val="1970019312"/>
+        <c:axId val="1970023664"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-516952208"/>
+        <c:axId val="1970019312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516951664"/>
+        <c:crossAx val="1970023664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1456,7 +1456,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-516951664"/>
+        <c:axId val="1970023664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1507,7 +1507,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516952208"/>
+        <c:crossAx val="1970019312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1710,64 +1710,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.726094766</c:v>
+                  <c:v>0.35758230499999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.65749425299999997</c:v>
+                  <c:v>0.42672908999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.64973596300000003</c:v>
+                  <c:v>0.47855314700000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.64921077400000005</c:v>
+                  <c:v>0.51514675099999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.64919084800000004</c:v>
+                  <c:v>0.54048734600000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.64918979399999999</c:v>
+                  <c:v>0.55801940699999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.57020912099999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.57873681799999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.58473984899999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.58899130200000005</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59202005000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59419021000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59575397100000005</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59688699499999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59771232299999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59831661300000005</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.64918979499999996</c:v>
+                  <c:v>0.59876123599999997</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.64918912699999998</c:v>
+                  <c:v>0.59908989999999995</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.64918912699999998</c:v>
+                  <c:v>0.599333903</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.64918912699999998</c:v>
+                  <c:v>0.59951578699999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,64 +1876,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.77923099500000004</c:v>
+                  <c:v>0.31503964899999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70308816299999999</c:v>
+                  <c:v>0.36578413900000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68276588800000004</c:v>
+                  <c:v>0.39589666400000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.67956310499999995</c:v>
+                  <c:v>0.41320470399999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67921149800000002</c:v>
+                  <c:v>0.42250754299999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.67917738299999997</c:v>
+                  <c:v>0.42729956099999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67918103200000002</c:v>
+                  <c:v>0.42971907100000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.679181005</c:v>
+                  <c:v>0.43093272199999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.67918100100000001</c:v>
+                  <c:v>0.43154235499999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.67918100000000003</c:v>
+                  <c:v>0.43185045399999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.67918100000000003</c:v>
+                  <c:v>0.43200755299999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.67918100000000003</c:v>
+                  <c:v>0.43208850399999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.67918100000000003</c:v>
+                  <c:v>0.43213069199999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.43215293399999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.43216479400000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.43217118700000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.43217466900000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.432176581</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.432177641</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.67918102800000002</c:v>
+                  <c:v>0.432178232</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2042,64 +2042,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.76195865500000004</c:v>
+                  <c:v>0.26969879899999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72159557299999999</c:v>
+                  <c:v>0.30764681500000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69852466599999996</c:v>
+                  <c:v>0.32358064399999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69120798500000002</c:v>
+                  <c:v>0.33052563800000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68939822799999995</c:v>
+                  <c:v>0.33342961799999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.688961508</c:v>
+                  <c:v>0.334592263</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68884653399999995</c:v>
+                  <c:v>0.33504539700000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68881520100000004</c:v>
+                  <c:v>0.33521960099999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.68884809199999997</c:v>
+                  <c:v>0.335286274</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.68886024999999995</c:v>
+                  <c:v>0.335311839</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.68885909499999998</c:v>
+                  <c:v>0.33532170300000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.68885867000000001</c:v>
+                  <c:v>0.33532554399999998</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.68885851899999995</c:v>
+                  <c:v>0.33532705499999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.68885846500000003</c:v>
+                  <c:v>0.335327657</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.68885844500000004</c:v>
+                  <c:v>0.33532789899999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.68885843800000002</c:v>
+                  <c:v>0.33532799699999999</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.68885843499999999</c:v>
+                  <c:v>0.33532803799999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.68885843400000002</c:v>
+                  <c:v>0.33532805399999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.68886019300000001</c:v>
+                  <c:v>0.33532806100000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.68886019300000001</c:v>
+                  <c:v>0.33532806399999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2208,64 +2208,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.69563969699999995</c:v>
+                  <c:v>0.22969467299999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70259632100000002</c:v>
+                  <c:v>0.25815946400000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.69399091599999996</c:v>
+                  <c:v>0.26703510000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68358019000000003</c:v>
+                  <c:v>0.26996840999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.67707563699999995</c:v>
+                  <c:v>0.27094858100000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.67343326199999998</c:v>
+                  <c:v>0.27127869199999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.67131917500000005</c:v>
+                  <c:v>0.27139038900000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.67006593000000003</c:v>
+                  <c:v>0.27142851699999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.669259987</c:v>
+                  <c:v>0.271441708</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.66882967400000004</c:v>
+                  <c:v>0.271446352</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.66853244099999998</c:v>
+                  <c:v>0.27144801899999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.66839808999999994</c:v>
+                  <c:v>0.27144863200000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.66829448599999997</c:v>
+                  <c:v>0.27144886099999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.66826145299999995</c:v>
+                  <c:v>0.27144894899999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.66825959599999996</c:v>
+                  <c:v>0.27144898299999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.66829000999999999</c:v>
+                  <c:v>0.27144899700000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.66828373699999999</c:v>
+                  <c:v>0.27144900300000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.66827689999999995</c:v>
+                  <c:v>0.27144900500000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.66827247599999995</c:v>
+                  <c:v>0.27144900599999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.66827026599999995</c:v>
+                  <c:v>0.27144900599999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2281,11 +2281,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-516953296"/>
-        <c:axId val="-516964720"/>
+        <c:axId val="1970014416"/>
+        <c:axId val="1970019856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-516953296"/>
+        <c:axId val="1970014416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2328,7 +2328,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516964720"/>
+        <c:crossAx val="1970019856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2336,10 +2336,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-516964720"/>
+        <c:axId val="1970019856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.64000000000000012"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2388,7 +2387,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516953296"/>
+        <c:crossAx val="1970014416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2591,64 +2590,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.980650036</c:v>
+                  <c:v>0.83271283299999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.93825375899999996</c:v>
+                  <c:v>0.70195786699999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.93053849799999999</c:v>
+                  <c:v>0.605480303</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92972328100000001</c:v>
+                  <c:v>0.53723485299999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.929684552</c:v>
+                  <c:v>0.48994965400000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.92967836299999995</c:v>
+                  <c:v>0.457230046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.43447976100000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.41856390100000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.40735997499999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.39942514800000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.39377235100000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.38972200600000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.38680343299999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.38468877899999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.38314840300000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.382020568</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.92967836100000001</c:v>
+                  <c:v>0.38119073199999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.92967836400000003</c:v>
+                  <c:v>0.38057732100000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.92967836400000003</c:v>
+                  <c:v>0.38012191699999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.92967836400000003</c:v>
+                  <c:v>0.37978245300000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2757,64 +2756,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.92058611199999996</c:v>
+                  <c:v>0.701066207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88725318799999997</c:v>
+                  <c:v>0.58501808399999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.87169902200000005</c:v>
+                  <c:v>0.51752624700000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86771158800000003</c:v>
+                  <c:v>0.47839593000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86704340599999996</c:v>
+                  <c:v>0.45727283400000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.866945615</c:v>
+                  <c:v>0.44636821799999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.866954844</c:v>
+                  <c:v>0.44085606999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86695420099999998</c:v>
+                  <c:v>0.43808936799999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.86695408299999999</c:v>
+                  <c:v>0.43669912500000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.86695406200000003</c:v>
+                  <c:v>0.43599637600000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.86695405800000003</c:v>
+                  <c:v>0.43563800499999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.86695405699999994</c:v>
+                  <c:v>0.43545333000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.86695405699999994</c:v>
+                  <c:v>0.43535708299999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43530633800000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43527927900000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43526469200000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43525675000000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43525238599999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.43524996799999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.86695502999999996</c:v>
+                  <c:v>0.435248619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2923,64 +2922,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.82840527399999997</c:v>
+                  <c:v>0.595737403</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.82306905100000005</c:v>
+                  <c:v>0.485106062</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.81183950299999996</c:v>
+                  <c:v>0.43977316700000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.80296807800000003</c:v>
+                  <c:v>0.41970744300000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.79922856099999995</c:v>
+                  <c:v>0.41122691</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.79802217600000003</c:v>
+                  <c:v>0.40780766299999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.79758105000000001</c:v>
+                  <c:v>0.406468571</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.79741544499999994</c:v>
+                  <c:v>0.40595194899999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.79749990500000001</c:v>
+                  <c:v>0.405753694</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79754134099999996</c:v>
+                  <c:v>0.40567751499999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.79753589199999997</c:v>
+                  <c:v>0.40564807200000003</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.79753387099999995</c:v>
+                  <c:v>0.40563659200000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.79753313400000003</c:v>
+                  <c:v>0.40563206899999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.79753286599999995</c:v>
+                  <c:v>0.40563026699999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.79753276699999998</c:v>
+                  <c:v>0.40562954099999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.79753273099999999</c:v>
+                  <c:v>0.405629246</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.79753271699999995</c:v>
+                  <c:v>0.40562912499999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.79753271199999998</c:v>
+                  <c:v>0.40562907500000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.79754003100000004</c:v>
+                  <c:v>0.40562905399999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.79754002999999996</c:v>
+                  <c:v>0.40562904500000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3089,64 +3088,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.72296543400000002</c:v>
+                  <c:v>0.50965847900000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.73764036499999996</c:v>
+                  <c:v>0.39933551099999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.74461753399999997</c:v>
+                  <c:v>0.36558017700000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.73035262899999998</c:v>
+                  <c:v>0.35427599999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.71596585700000004</c:v>
+                  <c:v>0.35043429100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70636421999999999</c:v>
+                  <c:v>0.349129413</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70032646899999995</c:v>
+                  <c:v>0.348685409</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.69654961299999996</c:v>
+                  <c:v>0.34853326800000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.694274218</c:v>
+                  <c:v>0.348480493</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.692845924</c:v>
+                  <c:v>0.348461878</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.69198630299999997</c:v>
+                  <c:v>0.34845518199999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.691523938</c:v>
+                  <c:v>0.34845271999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.69119294899999995</c:v>
+                  <c:v>0.34845179599999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.69104728800000004</c:v>
+                  <c:v>0.34845144099999997</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.69101715699999999</c:v>
+                  <c:v>0.34845130200000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.69107229400000003</c:v>
+                  <c:v>0.34845124700000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.69104395500000004</c:v>
+                  <c:v>0.34845122499999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.69102011900000004</c:v>
+                  <c:v>0.34845121600000001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.69100509600000004</c:v>
+                  <c:v>0.34845121299999998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.690997313</c:v>
+                  <c:v>0.34845121099999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3162,11 +3161,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-516957104"/>
-        <c:axId val="-516962544"/>
+        <c:axId val="1970025296"/>
+        <c:axId val="1970020944"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-516957104"/>
+        <c:axId val="1970025296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3209,7 +3208,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516962544"/>
+        <c:crossAx val="1970020944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3217,11 +3216,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-516962544"/>
+        <c:axId val="1970020944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1"/>
-          <c:min val="0.65000000000000013"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3270,7 +3267,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516957104"/>
+        <c:crossAx val="1970025296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3473,64 +3470,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.267415925</c:v>
+                  <c:v>0.52596712199999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.28378962299999999</c:v>
+                  <c:v>0.45999001900000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.28329694399999999</c:v>
+                  <c:v>0.39913509899999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28314011300000003</c:v>
+                  <c:v>0.35359056999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.28313070800000001</c:v>
+                  <c:v>0.32158660100000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.28312908399999998</c:v>
+                  <c:v>0.29935751999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.28388558600000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.27305854299999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.26543628800000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.26003795299999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.25619213899999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.25343652900000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.251450909</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.25001222499999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.248964246</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.24819693500000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.283129083</c:v>
+                  <c:v>0.24763236499999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.28312975099999999</c:v>
+                  <c:v>0.247215037</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.28312975099999999</c:v>
+                  <c:v>0.24690520699999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.28312975099999999</c:v>
+                  <c:v>0.24667425600000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3639,64 +3636,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.18736978500000001</c:v>
+                  <c:v>0.45914265300000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.20104085099999999</c:v>
+                  <c:v>0.394060509</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.201050583</c:v>
+                  <c:v>0.34916529499999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20058846499999999</c:v>
+                  <c:v>0.32000051600000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.200479186</c:v>
+                  <c:v>0.30346786999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.20046003400000001</c:v>
+                  <c:v>0.29473039899999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.20046164499999999</c:v>
+                  <c:v>0.29025980200000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.20046149399999999</c:v>
+                  <c:v>0.28800105199999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.200461466</c:v>
+                  <c:v>0.28686188699999998</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.20046146100000001</c:v>
+                  <c:v>0.28628486600000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.20046146000000001</c:v>
+                  <c:v>0.28599026500000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20046145900000001</c:v>
+                  <c:v>0.28583835000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20046145900000001</c:v>
+                  <c:v>0.28575914600000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28571737800000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28569510300000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28568309400000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28567655600000003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28567296199999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28567097200000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.20046145500000001</c:v>
+                  <c:v>0.28566986100000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3805,64 +3802,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.148672375</c:v>
+                  <c:v>0.40079779599999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14215206699999999</c:v>
+                  <c:v>0.32328309100000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.14079139900000001</c:v>
+                  <c:v>0.28881318099999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.139662909</c:v>
+                  <c:v>0.271629075</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13910614399999999</c:v>
+                  <c:v>0.26384175100000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.13890459699999999</c:v>
+                  <c:v>0.260566144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.13882782799999999</c:v>
+                  <c:v>0.25924710400000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.138799265</c:v>
+                  <c:v>0.25872812899999997</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13880811900000001</c:v>
+                  <c:v>0.25852605200000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.138813505</c:v>
+                  <c:v>0.25844752999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.13881253199999999</c:v>
+                  <c:v>0.25841691</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13881217200000001</c:v>
+                  <c:v>0.25840488499999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.13881204</c:v>
+                  <c:v>0.25840011800000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.138811992</c:v>
+                  <c:v>0.25839821000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.138811975</c:v>
+                  <c:v>0.25839743799999998</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13881196800000001</c:v>
+                  <c:v>0.25839712300000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13881196600000001</c:v>
+                  <c:v>0.25839699300000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.13881196500000001</c:v>
+                  <c:v>0.25839693899999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.13881262999999999</c:v>
+                  <c:v>0.258396917</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.13881262999999999</c:v>
+                  <c:v>0.25839690700000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3971,64 +3968,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>0.13339302</c:v>
+                  <c:v>0.346120494</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.101552237</c:v>
+                  <c:v>0.25358784899999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5899423999999997E-2</c:v>
+                  <c:v>0.22344106</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.3306976999999999E-2</c:v>
+                  <c:v>0.21244064300000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.1420151000000005E-2</c:v>
+                  <c:v>0.20849357099999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9.0177816999999993E-2</c:v>
+                  <c:v>0.20710684700000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.9392445000000001E-2</c:v>
+                  <c:v>0.206624945</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.8896958999999998E-2</c:v>
+                  <c:v>0.206457574</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.8599724000000005E-2</c:v>
+                  <c:v>0.206399002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.8412490999999996E-2</c:v>
+                  <c:v>0.206378222</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>8.8300043999999994E-2</c:v>
+                  <c:v>0.20637071800000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8.8236551999999996E-2</c:v>
+                  <c:v>0.20636795199999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.8193360999999998E-2</c:v>
+                  <c:v>0.20636691099999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8.8173197999999994E-2</c:v>
+                  <c:v>0.206366512</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.8167835999999999E-2</c:v>
+                  <c:v>0.206366356</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>8.8170603E-2</c:v>
+                  <c:v>0.20636629400000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.8166570999999999E-2</c:v>
+                  <c:v>0.20636626899999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.8163399000000003E-2</c:v>
+                  <c:v>0.206366259</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.8161404999999998E-2</c:v>
+                  <c:v>0.206366254</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.8160349999999998E-2</c:v>
+                  <c:v>0.206366253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4044,11 +4041,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-516962000"/>
-        <c:axId val="-516961456"/>
+        <c:axId val="1970025840"/>
+        <c:axId val="1970015504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-516962000"/>
+        <c:axId val="1970025840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4091,7 +4088,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516961456"/>
+        <c:crossAx val="1970015504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4099,11 +4096,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-516961456"/>
+        <c:axId val="1970015504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.30000000000000004"/>
-          <c:min val="5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4152,7 +4147,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-516962000"/>
+        <c:crossAx val="1970025840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7453,8 +7448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7481,16 +7476,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.89159839299999999</v>
+        <v>1.9047595879999999</v>
       </c>
       <c r="C2">
-        <v>0.84578794700000004</v>
+        <v>2.2202717750000001</v>
       </c>
       <c r="D2">
-        <v>0.98670907799999996</v>
+        <v>2.657843765</v>
       </c>
       <c r="E2">
-        <v>1.37887468</v>
+        <v>3.2033417790000001</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -7498,16 +7493,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.88649849000000003</v>
+        <v>1.6372711600000001</v>
       </c>
       <c r="C3">
-        <v>0.97297827100000001</v>
+        <v>1.906407704</v>
       </c>
       <c r="D3">
-        <v>0.80652002899999997</v>
+        <v>2.2476537969999999</v>
       </c>
       <c r="E3">
-        <v>1.3811905179999999</v>
+        <v>2.6667503739999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -7515,16 +7510,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.78476864599999996</v>
+        <v>1.443286721</v>
       </c>
       <c r="C4">
-        <v>0.92492790899999999</v>
+        <v>1.743074867</v>
       </c>
       <c r="D4">
-        <v>0.64205165799999997</v>
+        <v>2.1074637389999999</v>
       </c>
       <c r="E4">
-        <v>1.204372706</v>
+        <v>2.524938938</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -7532,16 +7527,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.71030030700000002</v>
+        <v>1.3056021710000001</v>
       </c>
       <c r="C5">
-        <v>0.88369139100000005</v>
+        <v>1.647882598</v>
       </c>
       <c r="D5">
-        <v>0.70602313999999999</v>
+        <v>2.0463224719999999</v>
       </c>
       <c r="E5">
-        <v>1.440764081</v>
+        <v>2.4776554640000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -7549,16 +7544,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.66031703399999997</v>
+        <v>1.2100407959999999</v>
       </c>
       <c r="C6">
-        <v>0.86093504899999995</v>
+        <v>1.5957947370000001</v>
       </c>
       <c r="D6">
-        <v>0.78627315600000003</v>
+        <v>2.0196704259999998</v>
       </c>
       <c r="E6">
-        <v>1.844072224</v>
+        <v>2.4614160730000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -7566,16 +7561,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.62660321699999999</v>
+        <v>1.1438732410000001</v>
       </c>
       <c r="C7">
-        <v>0.84941587900000004</v>
+        <v>1.568624631</v>
       </c>
       <c r="D7">
-        <v>0.82873205400000005</v>
+        <v>2.008500937</v>
       </c>
       <c r="E7">
-        <v>2.2140574040000001</v>
+        <v>2.4555925510000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -7583,16 +7578,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.60356510100000005</v>
+        <v>1.0978559349999999</v>
       </c>
       <c r="C8">
-        <v>0.84370419799999996</v>
+        <v>1.554790557</v>
       </c>
       <c r="D8">
-        <v>0.85049989800000003</v>
+        <v>2.0039550290000001</v>
       </c>
       <c r="E8">
-        <v>2.5082710459999999</v>
+        <v>2.4534809989999999</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -7600,16 +7595,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.58764697899999996</v>
+        <v>1.0656603090000001</v>
       </c>
       <c r="C9">
-        <v>0.84088365099999995</v>
+        <v>1.5478123669999999</v>
       </c>
       <c r="D9">
-        <v>0.86085452500000004</v>
+        <v>2.0021353679999998</v>
       </c>
       <c r="E9">
-        <v>2.732456209</v>
+        <v>2.452707856</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -7617,16 +7612,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.57654287900000001</v>
+        <v>1.042995737</v>
       </c>
       <c r="C10">
-        <v>0.83947799499999998</v>
+        <v>1.544294209</v>
       </c>
       <c r="D10">
-        <v>0.860258525</v>
+        <v>2.0014121490000001</v>
       </c>
       <c r="E10">
-        <v>2.8882100909999999</v>
+        <v>2.4524213750000001</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -7634,16 +7629,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.56872575199999997</v>
+        <v>1.0269441479999999</v>
       </c>
       <c r="C11">
-        <v>0.83876762500000002</v>
+        <v>1.5425119169999999</v>
       </c>
       <c r="D11">
-        <v>0.85933168999999998</v>
+        <v>2.0011248269999999</v>
       </c>
       <c r="E11">
-        <v>3.005277446</v>
+        <v>2.452313642</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -7651,16 +7646,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.56319391699999999</v>
+        <v>1.0155089150000001</v>
       </c>
       <c r="C12">
-        <v>0.83841194799999996</v>
+        <v>1.541601722</v>
       </c>
       <c r="D12">
-        <v>0.85985331799999998</v>
+        <v>2.0010101950000001</v>
       </c>
       <c r="E12">
-        <v>3.0821550680000001</v>
+        <v>2.4522724220000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -7668,16 +7663,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.55923497200000005</v>
+        <v>1.00731533</v>
       </c>
       <c r="C13">
-        <v>0.838229106</v>
+        <v>1.54113225</v>
       </c>
       <c r="D13">
-        <v>0.86006689300000005</v>
+        <v>2.0009641249999999</v>
       </c>
       <c r="E13">
-        <v>3.1349551029999998</v>
+        <v>2.4522563540000002</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -7685,16 +7680,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.55639856399999998</v>
+        <v>1.001411246</v>
       </c>
       <c r="C14">
-        <v>0.83814010400000005</v>
+        <v>1.5408874299999999</v>
       </c>
       <c r="D14">
-        <v>0.86015311500000002</v>
+        <v>2.0009454400000002</v>
       </c>
       <c r="E14">
-        <v>3.1725827290000002</v>
+        <v>2.4522499720000002</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -7702,16 +7697,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.55434677200000004</v>
+        <v>0.99713343600000004</v>
       </c>
       <c r="C15">
-        <v>0.83809098900000001</v>
+        <v>1.5407583060000001</v>
       </c>
       <c r="D15">
-        <v>0.86018769500000003</v>
+        <v>2.0009377879999999</v>
       </c>
       <c r="E15">
-        <v>3.196329843</v>
+        <v>2.4522473910000002</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -7719,16 +7714,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.55285921000000005</v>
+        <v>0.99401735400000002</v>
       </c>
       <c r="C16">
-        <v>0.83807003999999996</v>
+        <v>1.540689435</v>
       </c>
       <c r="D16">
-        <v>0.86020150299999998</v>
+        <v>2.000934623</v>
       </c>
       <c r="E16">
-        <v>3.2082232180000001</v>
+        <v>2.4522463299999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -7736,16 +7731,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.55177585600000001</v>
+        <v>0.99173581799999999</v>
       </c>
       <c r="C17">
-        <v>0.83805931300000003</v>
+        <v>1.540652304</v>
       </c>
       <c r="D17">
-        <v>0.86020701099999997</v>
+        <v>2.0009333030000001</v>
       </c>
       <c r="E17">
-        <v>3.2135334109999998</v>
+        <v>2.4522458889999998</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -7753,16 +7748,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.55097579600000002</v>
+        <v>0.99005711299999999</v>
       </c>
       <c r="C18">
-        <v>0.83805546600000003</v>
+        <v>1.5406320849999999</v>
       </c>
       <c r="D18">
-        <v>0.86020920000000001</v>
+        <v>2.0009327469999998</v>
       </c>
       <c r="E18">
-        <v>3.2201323629999998</v>
+        <v>2.452245703</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -7770,16 +7765,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.55039095699999996</v>
+        <v>0.98881622199999997</v>
       </c>
       <c r="C19">
-        <v>0.83805228799999998</v>
+        <v>1.5406209740000001</v>
       </c>
       <c r="D19">
-        <v>0.86021006499999997</v>
+        <v>2.000932513</v>
       </c>
       <c r="E19">
-        <v>3.2247391080000001</v>
+        <v>2.4522456240000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -7787,16 +7782,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.549955207</v>
+        <v>0.98789496899999996</v>
       </c>
       <c r="C20">
-        <v>0.83805280800000004</v>
+        <v>1.540614819</v>
       </c>
       <c r="D20">
-        <v>0.860009001</v>
+        <v>2.0009324130000001</v>
       </c>
       <c r="E20">
-        <v>3.2278067240000001</v>
+        <v>2.45224559</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -7804,16 +7799,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.54963043499999997</v>
+        <v>0.98720825499999998</v>
       </c>
       <c r="C21">
-        <v>0.83805343700000001</v>
+        <v>1.540611384</v>
       </c>
       <c r="D21">
-        <v>0.86000913300000004</v>
+        <v>2.0009323700000001</v>
       </c>
       <c r="E21">
-        <v>3.2297245440000002</v>
+        <v>2.4522455760000001</v>
       </c>
     </row>
   </sheetData>
@@ -7827,7 +7822,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7854,16 +7849,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.12860655100000001</v>
+        <v>0.16728716599999999</v>
       </c>
       <c r="C2">
-        <v>0.50616134999999995</v>
+        <v>0.29893379199999998</v>
       </c>
       <c r="D2">
-        <v>0.98670907799999996</v>
+        <v>0.40426259599999997</v>
       </c>
       <c r="E2">
-        <v>1.37887468</v>
+        <v>0.49034151999999998</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -7871,16 +7866,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>4.0159904000000003E-2</v>
+        <v>0.34014248000000002</v>
       </c>
       <c r="C3">
-        <v>0.29139865700000001</v>
+        <v>0.51668483799999998</v>
       </c>
       <c r="D3">
-        <v>0.80652002899999997</v>
+        <v>0.69034385600000003</v>
       </c>
       <c r="E3">
-        <v>1.3811905179999999</v>
+        <v>0.86019787400000003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -7888,16 +7883,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>3.0761482E-2</v>
+        <v>0.58845096799999996</v>
       </c>
       <c r="C4">
-        <v>0.22048114799999999</v>
+        <v>0.74617820000000001</v>
       </c>
       <c r="D4">
-        <v>0.64205165799999997</v>
+        <v>0.92072630899999997</v>
       </c>
       <c r="E4">
-        <v>1.204372706</v>
+        <v>1.1304277899999999</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -7905,16 +7900,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>3.2080589E-2</v>
+        <v>0.887835441</v>
       </c>
       <c r="C5">
-        <v>0.229747388</v>
+        <v>0.98713218300000005</v>
       </c>
       <c r="D5">
-        <v>0.70602313999999999</v>
+        <v>1.118072161</v>
       </c>
       <c r="E5">
-        <v>1.440764081</v>
+        <v>1.3266246399999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -7922,16 +7917,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>3.2148706999999999E-2</v>
+        <v>1.209767939</v>
       </c>
       <c r="C6">
-        <v>0.23700928900000001</v>
+        <v>1.216379541</v>
       </c>
       <c r="D6">
-        <v>0.78627315600000003</v>
+        <v>1.2833249790000001</v>
       </c>
       <c r="E6">
-        <v>1.844072224</v>
+        <v>1.4702520640000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -7939,16 +7934,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>3.2215292E-2</v>
+        <v>1.535671896</v>
       </c>
       <c r="C7">
-        <v>0.23909171700000001</v>
+        <v>1.4212518590000001</v>
       </c>
       <c r="D7">
-        <v>0.82873205400000005</v>
+        <v>1.418161303</v>
       </c>
       <c r="E7">
-        <v>2.2140574040000001</v>
+        <v>1.577077214</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -7956,16 +7951,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>3.221537E-2</v>
+        <v>1.854602343</v>
       </c>
       <c r="C8">
-        <v>0.23905536499999999</v>
+        <v>1.5989392499999999</v>
       </c>
       <c r="D8">
-        <v>0.85049989800000003</v>
+        <v>1.5271453989999999</v>
       </c>
       <c r="E8">
-        <v>2.5082710459999999</v>
+        <v>1.6580968410000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -7973,16 +7968,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>3.2215375999999997E-2</v>
+        <v>2.1605089030000002</v>
       </c>
       <c r="C9">
-        <v>0.239102747</v>
+        <v>1.7513704590000001</v>
       </c>
       <c r="D9">
-        <v>0.86085452500000004</v>
+        <v>1.615515313</v>
       </c>
       <c r="E9">
-        <v>2.732456209</v>
+        <v>1.720868646</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -7990,16 +7985,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>3.2215375999999997E-2</v>
+        <v>2.4504152719999999</v>
       </c>
       <c r="C10">
-        <v>0.23911279999999999</v>
+        <v>1.8820732120000001</v>
       </c>
       <c r="D10">
-        <v>0.860258525</v>
+        <v>1.6879366499999999</v>
       </c>
       <c r="E10">
-        <v>2.8882100909999999</v>
+        <v>1.7706135119999999</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -8007,16 +8002,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>3.2215375999999997E-2</v>
+        <v>2.7232547820000002</v>
       </c>
       <c r="C11">
-        <v>0.23911487100000001</v>
+        <v>1.9947453639999999</v>
       </c>
       <c r="D11">
-        <v>0.85933168999999998</v>
+        <v>1.7481742069999999</v>
       </c>
       <c r="E11">
-        <v>3.005277446</v>
+        <v>1.8109810289999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -8024,16 +8019,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>3.2215375999999997E-2</v>
+        <v>2.9791196590000002</v>
       </c>
       <c r="C12">
-        <v>0.239115296</v>
+        <v>2.0927140569999998</v>
       </c>
       <c r="D12">
-        <v>0.85985331799999998</v>
+        <v>1.7991414450000001</v>
       </c>
       <c r="E12">
-        <v>3.0821550680000001</v>
+        <v>1.84455076</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -8041,16 +8036,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>3.2215375999999997E-2</v>
+        <v>3.218774233</v>
       </c>
       <c r="C13">
-        <v>0.23911538299999999</v>
+        <v>2.178787942</v>
       </c>
       <c r="D13">
-        <v>0.86006689300000005</v>
+        <v>1.843052403</v>
       </c>
       <c r="E13">
-        <v>3.1349551029999998</v>
+        <v>1.8731605419999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -8058,16 +8053,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>3.2215375999999997E-2</v>
+        <v>3.4433406030000002</v>
       </c>
       <c r="C14">
-        <v>0.23911540000000001</v>
+        <v>2.2552662379999999</v>
       </c>
       <c r="D14">
-        <v>0.86015311500000002</v>
+        <v>1.88157643</v>
       </c>
       <c r="E14">
-        <v>3.1725827290000002</v>
+        <v>1.898126457</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -8075,16 +8070,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>3.2215375999999997E-2</v>
+        <v>3.6540984380000001</v>
       </c>
       <c r="C15">
-        <v>0.23910288299999999</v>
+        <v>2.3240015380000001</v>
       </c>
       <c r="D15">
-        <v>0.86018769500000003</v>
+        <v>1.9159680690000001</v>
       </c>
       <c r="E15">
-        <v>3.196329843</v>
+        <v>1.9203939569999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -8092,16 +8087,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>3.2215375999999997E-2</v>
+        <v>3.8523605839999999</v>
       </c>
       <c r="C16">
-        <v>0.23910288299999999</v>
+        <v>2.3864740229999999</v>
       </c>
       <c r="D16">
-        <v>0.86020150299999998</v>
+        <v>1.9471690239999999</v>
       </c>
       <c r="E16">
-        <v>3.2082232180000001</v>
+        <v>1.9406436460000001</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -8109,16 +8104,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>3.2215375999999997E-2</v>
+        <v>4.0393987989999998</v>
       </c>
       <c r="C17">
-        <v>0.23910288399999999</v>
+        <v>2.443860999</v>
       </c>
       <c r="D17">
-        <v>0.86020701099999997</v>
+        <v>1.975886056</v>
       </c>
       <c r="E17">
-        <v>3.2135334109999998</v>
+        <v>1.959366242</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -8126,16 +8121,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>3.2215375999999997E-2</v>
+        <v>4.2164022719999998</v>
       </c>
       <c r="C18">
-        <v>0.23910288399999999</v>
+        <v>2.497096703</v>
       </c>
       <c r="D18">
-        <v>0.86020920000000001</v>
+        <v>2.0026498290000001</v>
       </c>
       <c r="E18">
-        <v>3.2201323629999998</v>
+        <v>1.9769160539999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -8143,16 +8138,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>3.2215343E-2</v>
+        <v>4.384457287</v>
       </c>
       <c r="C19">
-        <v>0.23910288399999999</v>
+        <v>2.5469217209999999</v>
       </c>
       <c r="D19">
-        <v>0.86021006499999997</v>
+        <v>2.0278591129999999</v>
       </c>
       <c r="E19">
-        <v>3.2247391080000001</v>
+        <v>1.9935493129999999</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -8160,16 +8155,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>3.2215343E-2</v>
+        <v>4.5445401710000004</v>
       </c>
       <c r="C20">
-        <v>0.23910288399999999</v>
+        <v>2.5939230100000001</v>
       </c>
       <c r="D20">
-        <v>0.860009001</v>
+        <v>2.0518139340000001</v>
       </c>
       <c r="E20">
-        <v>3.2278067240000001</v>
+        <v>2.0094516809999998</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -8177,16 +8172,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>3.2215343E-2</v>
+        <v>4.6975183530000004</v>
       </c>
       <c r="C21">
-        <v>0.23910288399999999</v>
+        <v>2.6385659330000002</v>
       </c>
       <c r="D21">
-        <v>0.86000913300000004</v>
+        <v>2.0747403879999999</v>
       </c>
       <c r="E21">
-        <v>3.2297245440000002</v>
+        <v>2.024758024</v>
       </c>
     </row>
   </sheetData>
@@ -8201,7 +8196,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8228,16 +8223,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.726094766</v>
+        <v>0.35758230499999999</v>
       </c>
       <c r="C2">
-        <v>0.77923099500000004</v>
+        <v>0.31503964899999998</v>
       </c>
       <c r="D2">
-        <v>0.76195865500000004</v>
+        <v>0.26969879899999999</v>
       </c>
       <c r="E2">
-        <v>0.69563969699999995</v>
+        <v>0.22969467299999999</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8245,16 +8240,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.65749425299999997</v>
+        <v>0.42672908999999998</v>
       </c>
       <c r="C3">
-        <v>0.70308816299999999</v>
+        <v>0.36578413900000001</v>
       </c>
       <c r="D3">
-        <v>0.72159557299999999</v>
+        <v>0.30764681500000002</v>
       </c>
       <c r="E3">
-        <v>0.70259632100000002</v>
+        <v>0.25815946400000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -8262,16 +8257,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.64973596300000003</v>
+        <v>0.47855314700000001</v>
       </c>
       <c r="C4">
-        <v>0.68276588800000004</v>
+        <v>0.39589666400000001</v>
       </c>
       <c r="D4">
-        <v>0.69852466599999996</v>
+        <v>0.32358064399999997</v>
       </c>
       <c r="E4">
-        <v>0.69399091599999996</v>
+        <v>0.26703510000000003</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -8279,16 +8274,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.64921077400000005</v>
+        <v>0.51514675099999996</v>
       </c>
       <c r="C5">
-        <v>0.67956310499999995</v>
+        <v>0.41320470399999998</v>
       </c>
       <c r="D5">
-        <v>0.69120798500000002</v>
+        <v>0.33052563800000001</v>
       </c>
       <c r="E5">
-        <v>0.68358019000000003</v>
+        <v>0.26996840999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -8296,16 +8291,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.64919084800000004</v>
+        <v>0.54048734600000004</v>
       </c>
       <c r="C6">
-        <v>0.67921149800000002</v>
+        <v>0.42250754299999999</v>
       </c>
       <c r="D6">
-        <v>0.68939822799999995</v>
+        <v>0.33342961799999998</v>
       </c>
       <c r="E6">
-        <v>0.67707563699999995</v>
+        <v>0.27094858100000002</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -8313,16 +8308,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.64918979399999999</v>
+        <v>0.55801940699999997</v>
       </c>
       <c r="C7">
-        <v>0.67917738299999997</v>
+        <v>0.42729956099999999</v>
       </c>
       <c r="D7">
-        <v>0.688961508</v>
+        <v>0.334592263</v>
       </c>
       <c r="E7">
-        <v>0.67343326199999998</v>
+        <v>0.27127869199999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -8330,16 +8325,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.64918979499999996</v>
+        <v>0.57020912099999999</v>
       </c>
       <c r="C8">
-        <v>0.67918103200000002</v>
+        <v>0.42971907100000001</v>
       </c>
       <c r="D8">
-        <v>0.68884653399999995</v>
+        <v>0.33504539700000002</v>
       </c>
       <c r="E8">
-        <v>0.67131917500000005</v>
+        <v>0.27139038900000001</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -8347,16 +8342,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.64918979499999996</v>
+        <v>0.57873681799999999</v>
       </c>
       <c r="C9">
-        <v>0.679181005</v>
+        <v>0.43093272199999999</v>
       </c>
       <c r="D9">
-        <v>0.68881520100000004</v>
+        <v>0.33521960099999998</v>
       </c>
       <c r="E9">
-        <v>0.67006593000000003</v>
+        <v>0.27142851699999998</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -8364,16 +8359,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.64918979499999996</v>
+        <v>0.58473984899999998</v>
       </c>
       <c r="C10">
-        <v>0.67918100100000001</v>
+        <v>0.43154235499999999</v>
       </c>
       <c r="D10">
-        <v>0.68884809199999997</v>
+        <v>0.335286274</v>
       </c>
       <c r="E10">
-        <v>0.669259987</v>
+        <v>0.271441708</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -8381,16 +8376,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.64918979499999996</v>
+        <v>0.58899130200000005</v>
       </c>
       <c r="C11">
-        <v>0.67918100000000003</v>
+        <v>0.43185045399999999</v>
       </c>
       <c r="D11">
-        <v>0.68886024999999995</v>
+        <v>0.335311839</v>
       </c>
       <c r="E11">
-        <v>0.66882967400000004</v>
+        <v>0.271446352</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -8398,16 +8393,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.64918979499999996</v>
+        <v>0.59202005000000002</v>
       </c>
       <c r="C12">
-        <v>0.67918100000000003</v>
+        <v>0.43200755299999999</v>
       </c>
       <c r="D12">
-        <v>0.68885909499999998</v>
+        <v>0.33532170300000003</v>
       </c>
       <c r="E12">
-        <v>0.66853244099999998</v>
+        <v>0.27144801899999998</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -8415,16 +8410,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.64918979499999996</v>
+        <v>0.59419021000000005</v>
       </c>
       <c r="C13">
-        <v>0.67918100000000003</v>
+        <v>0.43208850399999998</v>
       </c>
       <c r="D13">
-        <v>0.68885867000000001</v>
+        <v>0.33532554399999998</v>
       </c>
       <c r="E13">
-        <v>0.66839808999999994</v>
+        <v>0.27144863200000002</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -8432,16 +8427,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.64918979499999996</v>
+        <v>0.59575397100000005</v>
       </c>
       <c r="C14">
-        <v>0.67918100000000003</v>
+        <v>0.43213069199999998</v>
       </c>
       <c r="D14">
-        <v>0.68885851899999995</v>
+        <v>0.33532705499999998</v>
       </c>
       <c r="E14">
-        <v>0.66829448599999997</v>
+        <v>0.27144886099999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -8449,16 +8444,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.64918979499999996</v>
+        <v>0.59688699499999998</v>
       </c>
       <c r="C15">
-        <v>0.67918102800000002</v>
+        <v>0.43215293399999999</v>
       </c>
       <c r="D15">
-        <v>0.68885846500000003</v>
+        <v>0.335327657</v>
       </c>
       <c r="E15">
-        <v>0.66826145299999995</v>
+        <v>0.27144894899999999</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -8466,16 +8461,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.64918979499999996</v>
+        <v>0.59771232299999999</v>
       </c>
       <c r="C16">
-        <v>0.67918102800000002</v>
+        <v>0.43216479400000002</v>
       </c>
       <c r="D16">
-        <v>0.68885844500000004</v>
+        <v>0.33532789899999998</v>
       </c>
       <c r="E16">
-        <v>0.66825959599999996</v>
+        <v>0.27144898299999998</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -8483,16 +8478,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.64918979499999996</v>
+        <v>0.59831661300000005</v>
       </c>
       <c r="C17">
-        <v>0.67918102800000002</v>
+        <v>0.43217118700000001</v>
       </c>
       <c r="D17">
-        <v>0.68885843800000002</v>
+        <v>0.33532799699999999</v>
       </c>
       <c r="E17">
-        <v>0.66829000999999999</v>
+        <v>0.27144899700000003</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -8500,16 +8495,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.64918979499999996</v>
+        <v>0.59876123599999997</v>
       </c>
       <c r="C18">
-        <v>0.67918102800000002</v>
+        <v>0.43217466900000001</v>
       </c>
       <c r="D18">
-        <v>0.68885843499999999</v>
+        <v>0.33532803799999999</v>
       </c>
       <c r="E18">
-        <v>0.66828373699999999</v>
+        <v>0.27144900300000002</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -8517,16 +8512,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.64918912699999998</v>
+        <v>0.59908989999999995</v>
       </c>
       <c r="C19">
-        <v>0.67918102800000002</v>
+        <v>0.432176581</v>
       </c>
       <c r="D19">
-        <v>0.68885843400000002</v>
+        <v>0.33532805399999999</v>
       </c>
       <c r="E19">
-        <v>0.66827689999999995</v>
+        <v>0.27144900500000002</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -8534,16 +8529,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.64918912699999998</v>
+        <v>0.599333903</v>
       </c>
       <c r="C20">
-        <v>0.67918102800000002</v>
+        <v>0.432177641</v>
       </c>
       <c r="D20">
-        <v>0.68886019300000001</v>
+        <v>0.33532806100000001</v>
       </c>
       <c r="E20">
-        <v>0.66827247599999995</v>
+        <v>0.27144900599999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -8551,16 +8546,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.64918912699999998</v>
+        <v>0.59951578699999997</v>
       </c>
       <c r="C21">
-        <v>0.67918102800000002</v>
+        <v>0.432178232</v>
       </c>
       <c r="D21">
-        <v>0.68886019300000001</v>
+        <v>0.33532806399999998</v>
       </c>
       <c r="E21">
-        <v>0.66827026599999995</v>
+        <v>0.27144900599999999</v>
       </c>
     </row>
   </sheetData>
@@ -8575,7 +8570,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8602,16 +8597,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.980650036</v>
+        <v>0.83271283299999999</v>
       </c>
       <c r="C2">
-        <v>0.92058611199999996</v>
+        <v>0.701066207</v>
       </c>
       <c r="D2">
-        <v>0.82840527399999997</v>
+        <v>0.595737403</v>
       </c>
       <c r="E2">
-        <v>0.72296543400000002</v>
+        <v>0.50965847900000005</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8619,16 +8614,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.93825375899999996</v>
+        <v>0.70195786699999996</v>
       </c>
       <c r="C3">
-        <v>0.88725318799999997</v>
+        <v>0.58501808399999999</v>
       </c>
       <c r="D3">
-        <v>0.82306905100000005</v>
+        <v>0.485106062</v>
       </c>
       <c r="E3">
-        <v>0.73764036499999996</v>
+        <v>0.39933551099999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -8636,16 +8631,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.93053849799999999</v>
+        <v>0.605480303</v>
       </c>
       <c r="C4">
-        <v>0.87169902200000005</v>
+        <v>0.51752624700000005</v>
       </c>
       <c r="D4">
-        <v>0.81183950299999996</v>
+        <v>0.43977316700000002</v>
       </c>
       <c r="E4">
-        <v>0.74461753399999997</v>
+        <v>0.36558017700000001</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -8653,16 +8648,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.92972328100000001</v>
+        <v>0.53723485299999996</v>
       </c>
       <c r="C5">
-        <v>0.86771158800000003</v>
+        <v>0.47839593000000002</v>
       </c>
       <c r="D5">
-        <v>0.80296807800000003</v>
+        <v>0.41970744300000001</v>
       </c>
       <c r="E5">
-        <v>0.73035262899999998</v>
+        <v>0.35427599999999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -8670,16 +8665,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.929684552</v>
+        <v>0.48994965400000001</v>
       </c>
       <c r="C6">
-        <v>0.86704340599999996</v>
+        <v>0.45727283400000002</v>
       </c>
       <c r="D6">
-        <v>0.79922856099999995</v>
+        <v>0.41122691</v>
       </c>
       <c r="E6">
-        <v>0.71596585700000004</v>
+        <v>0.35043429100000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -8687,16 +8682,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.92967836299999995</v>
+        <v>0.457230046</v>
       </c>
       <c r="C7">
-        <v>0.866945615</v>
+        <v>0.44636821799999998</v>
       </c>
       <c r="D7">
-        <v>0.79802217600000003</v>
+        <v>0.40780766299999999</v>
       </c>
       <c r="E7">
-        <v>0.70636421999999999</v>
+        <v>0.349129413</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -8704,16 +8699,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.92967836100000001</v>
+        <v>0.43447976100000002</v>
       </c>
       <c r="C8">
-        <v>0.866954844</v>
+        <v>0.44085606999999999</v>
       </c>
       <c r="D8">
-        <v>0.79758105000000001</v>
+        <v>0.406468571</v>
       </c>
       <c r="E8">
-        <v>0.70032646899999995</v>
+        <v>0.348685409</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -8721,16 +8716,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.92967836100000001</v>
+        <v>0.41856390100000002</v>
       </c>
       <c r="C9">
-        <v>0.86695420099999998</v>
+        <v>0.43808936799999998</v>
       </c>
       <c r="D9">
-        <v>0.79741544499999994</v>
+        <v>0.40595194899999998</v>
       </c>
       <c r="E9">
-        <v>0.69654961299999996</v>
+        <v>0.34853326800000001</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -8738,16 +8733,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.92967836100000001</v>
+        <v>0.40735997499999999</v>
       </c>
       <c r="C10">
-        <v>0.86695408299999999</v>
+        <v>0.43669912500000002</v>
       </c>
       <c r="D10">
-        <v>0.79749990500000001</v>
+        <v>0.405753694</v>
       </c>
       <c r="E10">
-        <v>0.694274218</v>
+        <v>0.348480493</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -8755,16 +8750,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.92967836100000001</v>
+        <v>0.39942514800000001</v>
       </c>
       <c r="C11">
-        <v>0.86695406200000003</v>
+        <v>0.43599637600000002</v>
       </c>
       <c r="D11">
-        <v>0.79754134099999996</v>
+        <v>0.40567751499999999</v>
       </c>
       <c r="E11">
-        <v>0.692845924</v>
+        <v>0.348461878</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -8772,16 +8767,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.92967836100000001</v>
+        <v>0.39377235100000002</v>
       </c>
       <c r="C12">
-        <v>0.86695405800000003</v>
+        <v>0.43563800499999999</v>
       </c>
       <c r="D12">
-        <v>0.79753589199999997</v>
+        <v>0.40564807200000003</v>
       </c>
       <c r="E12">
-        <v>0.69198630299999997</v>
+        <v>0.34845518199999997</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -8789,16 +8784,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.92967836100000001</v>
+        <v>0.38972200600000001</v>
       </c>
       <c r="C13">
-        <v>0.86695405699999994</v>
+        <v>0.43545333000000003</v>
       </c>
       <c r="D13">
-        <v>0.79753387099999995</v>
+        <v>0.40563659200000002</v>
       </c>
       <c r="E13">
-        <v>0.691523938</v>
+        <v>0.34845271999999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -8806,16 +8801,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.92967836100000001</v>
+        <v>0.38680343299999997</v>
       </c>
       <c r="C14">
-        <v>0.86695405699999994</v>
+        <v>0.43535708299999998</v>
       </c>
       <c r="D14">
-        <v>0.79753313400000003</v>
+        <v>0.40563206899999998</v>
       </c>
       <c r="E14">
-        <v>0.69119294899999995</v>
+        <v>0.34845179599999998</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -8823,16 +8818,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.92967836100000001</v>
+        <v>0.38468877899999998</v>
       </c>
       <c r="C15">
-        <v>0.86695502999999996</v>
+        <v>0.43530633800000001</v>
       </c>
       <c r="D15">
-        <v>0.79753286599999995</v>
+        <v>0.40563026699999999</v>
       </c>
       <c r="E15">
-        <v>0.69104728800000004</v>
+        <v>0.34845144099999997</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -8840,16 +8835,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.92967836100000001</v>
+        <v>0.38314840300000003</v>
       </c>
       <c r="C16">
-        <v>0.86695502999999996</v>
+        <v>0.43527927900000002</v>
       </c>
       <c r="D16">
-        <v>0.79753276699999998</v>
+        <v>0.40562954099999998</v>
       </c>
       <c r="E16">
-        <v>0.69101715699999999</v>
+        <v>0.34845130200000002</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -8857,16 +8852,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.92967836100000001</v>
+        <v>0.382020568</v>
       </c>
       <c r="C17">
-        <v>0.86695502999999996</v>
+        <v>0.43526469200000001</v>
       </c>
       <c r="D17">
-        <v>0.79753273099999999</v>
+        <v>0.405629246</v>
       </c>
       <c r="E17">
-        <v>0.69107229400000003</v>
+        <v>0.34845124700000002</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -8874,16 +8869,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.92967836100000001</v>
+        <v>0.38119073199999998</v>
       </c>
       <c r="C18">
-        <v>0.86695502999999996</v>
+        <v>0.43525675000000003</v>
       </c>
       <c r="D18">
-        <v>0.79753271699999995</v>
+        <v>0.40562912499999998</v>
       </c>
       <c r="E18">
-        <v>0.69104395500000004</v>
+        <v>0.34845122499999998</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -8891,16 +8886,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.92967836400000003</v>
+        <v>0.38057732100000002</v>
       </c>
       <c r="C19">
-        <v>0.86695502999999996</v>
+        <v>0.43525238599999999</v>
       </c>
       <c r="D19">
-        <v>0.79753271199999998</v>
+        <v>0.40562907500000001</v>
       </c>
       <c r="E19">
-        <v>0.69102011900000004</v>
+        <v>0.34845121600000001</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -8908,16 +8903,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.92967836400000003</v>
+        <v>0.38012191699999998</v>
       </c>
       <c r="C20">
-        <v>0.86695502999999996</v>
+        <v>0.43524996799999999</v>
       </c>
       <c r="D20">
-        <v>0.79754003100000004</v>
+        <v>0.40562905399999999</v>
       </c>
       <c r="E20">
-        <v>0.69100509600000004</v>
+        <v>0.34845121299999998</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -8925,16 +8920,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.92967836400000003</v>
+        <v>0.37978245300000002</v>
       </c>
       <c r="C21">
-        <v>0.86695502999999996</v>
+        <v>0.435248619</v>
       </c>
       <c r="D21">
-        <v>0.79754002999999996</v>
+        <v>0.40562904500000002</v>
       </c>
       <c r="E21">
-        <v>0.690997313</v>
+        <v>0.34845121099999998</v>
       </c>
     </row>
   </sheetData>
@@ -8948,8 +8943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8976,16 +8971,16 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.267415925</v>
+        <v>0.52596712199999995</v>
       </c>
       <c r="C2">
-        <v>0.18736978500000001</v>
+        <v>0.45914265300000001</v>
       </c>
       <c r="D2">
-        <v>0.148672375</v>
+        <v>0.40079779599999998</v>
       </c>
       <c r="E2">
-        <v>0.13339302</v>
+        <v>0.346120494</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -8993,16 +8988,16 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.28378962299999999</v>
+        <v>0.45999001900000003</v>
       </c>
       <c r="C3">
-        <v>0.20104085099999999</v>
+        <v>0.394060509</v>
       </c>
       <c r="D3">
-        <v>0.14215206699999999</v>
+        <v>0.32328309100000002</v>
       </c>
       <c r="E3">
-        <v>0.101552237</v>
+        <v>0.25358784899999998</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -9010,16 +9005,16 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.28329694399999999</v>
+        <v>0.39913509899999999</v>
       </c>
       <c r="C4">
-        <v>0.201050583</v>
+        <v>0.34916529499999999</v>
       </c>
       <c r="D4">
-        <v>0.14079139900000001</v>
+        <v>0.28881318099999997</v>
       </c>
       <c r="E4">
-        <v>9.5899423999999997E-2</v>
+        <v>0.22344106</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -9027,16 +9022,16 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.28314011300000003</v>
+        <v>0.35359056999999999</v>
       </c>
       <c r="C5">
-        <v>0.20058846499999999</v>
+        <v>0.32000051600000001</v>
       </c>
       <c r="D5">
-        <v>0.139662909</v>
+        <v>0.271629075</v>
       </c>
       <c r="E5">
-        <v>9.3306976999999999E-2</v>
+        <v>0.21244064300000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -9044,16 +9039,16 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.28313070800000001</v>
+        <v>0.32158660100000003</v>
       </c>
       <c r="C6">
-        <v>0.200479186</v>
+        <v>0.30346786999999997</v>
       </c>
       <c r="D6">
-        <v>0.13910614399999999</v>
+        <v>0.26384175100000001</v>
       </c>
       <c r="E6">
-        <v>9.1420151000000005E-2</v>
+        <v>0.20849357099999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -9061,16 +9056,16 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0.28312908399999998</v>
+        <v>0.29935751999999999</v>
       </c>
       <c r="C7">
-        <v>0.20046003400000001</v>
+        <v>0.29473039899999998</v>
       </c>
       <c r="D7">
-        <v>0.13890459699999999</v>
+        <v>0.260566144</v>
       </c>
       <c r="E7">
-        <v>9.0177816999999993E-2</v>
+        <v>0.20710684700000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -9078,16 +9073,16 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.283129083</v>
+        <v>0.28388558600000002</v>
       </c>
       <c r="C8">
-        <v>0.20046164499999999</v>
+        <v>0.29025980200000001</v>
       </c>
       <c r="D8">
-        <v>0.13882782799999999</v>
+        <v>0.25924710400000001</v>
       </c>
       <c r="E8">
-        <v>8.9392445000000001E-2</v>
+        <v>0.206624945</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -9095,16 +9090,16 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0.283129083</v>
+        <v>0.27305854299999999</v>
       </c>
       <c r="C9">
-        <v>0.20046149399999999</v>
+        <v>0.28800105199999998</v>
       </c>
       <c r="D9">
-        <v>0.138799265</v>
+        <v>0.25872812899999997</v>
       </c>
       <c r="E9">
-        <v>8.8896958999999998E-2</v>
+        <v>0.206457574</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -9112,16 +9107,16 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>0.283129083</v>
+        <v>0.26543628800000002</v>
       </c>
       <c r="C10">
-        <v>0.200461466</v>
+        <v>0.28686188699999998</v>
       </c>
       <c r="D10">
-        <v>0.13880811900000001</v>
+        <v>0.25852605200000001</v>
       </c>
       <c r="E10">
-        <v>8.8599724000000005E-2</v>
+        <v>0.206399002</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -9129,16 +9124,16 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>0.283129083</v>
+        <v>0.26003795299999999</v>
       </c>
       <c r="C11">
-        <v>0.20046146100000001</v>
+        <v>0.28628486600000003</v>
       </c>
       <c r="D11">
-        <v>0.138813505</v>
+        <v>0.25844752999999998</v>
       </c>
       <c r="E11">
-        <v>8.8412490999999996E-2</v>
+        <v>0.206378222</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -9146,16 +9141,16 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>0.283129083</v>
+        <v>0.25619213899999999</v>
       </c>
       <c r="C12">
-        <v>0.20046146000000001</v>
+        <v>0.28599026500000002</v>
       </c>
       <c r="D12">
-        <v>0.13881253199999999</v>
+        <v>0.25841691</v>
       </c>
       <c r="E12">
-        <v>8.8300043999999994E-2</v>
+        <v>0.20637071800000001</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -9163,16 +9158,16 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>0.283129083</v>
+        <v>0.25343652900000002</v>
       </c>
       <c r="C13">
-        <v>0.20046145900000001</v>
+        <v>0.28583835000000002</v>
       </c>
       <c r="D13">
-        <v>0.13881217200000001</v>
+        <v>0.25840488499999997</v>
       </c>
       <c r="E13">
-        <v>8.8236551999999996E-2</v>
+        <v>0.20636795199999999</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -9180,16 +9175,16 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>0.283129083</v>
+        <v>0.251450909</v>
       </c>
       <c r="C14">
-        <v>0.20046145900000001</v>
+        <v>0.28575914600000002</v>
       </c>
       <c r="D14">
-        <v>0.13881204</v>
+        <v>0.25840011800000001</v>
       </c>
       <c r="E14">
-        <v>8.8193360999999998E-2</v>
+        <v>0.20636691099999999</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -9197,16 +9192,16 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>0.283129083</v>
+        <v>0.25001222499999998</v>
       </c>
       <c r="C15">
-        <v>0.20046145500000001</v>
+        <v>0.28571737800000002</v>
       </c>
       <c r="D15">
-        <v>0.138811992</v>
+        <v>0.25839821000000002</v>
       </c>
       <c r="E15">
-        <v>8.8173197999999994E-2</v>
+        <v>0.206366512</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -9214,16 +9209,16 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>0.283129083</v>
+        <v>0.248964246</v>
       </c>
       <c r="C16">
-        <v>0.20046145500000001</v>
+        <v>0.28569510300000001</v>
       </c>
       <c r="D16">
-        <v>0.138811975</v>
+        <v>0.25839743799999998</v>
       </c>
       <c r="E16">
-        <v>8.8167835999999999E-2</v>
+        <v>0.206366356</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -9231,16 +9226,16 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>0.283129083</v>
+        <v>0.24819693500000001</v>
       </c>
       <c r="C17">
-        <v>0.20046145500000001</v>
+        <v>0.28568309400000003</v>
       </c>
       <c r="D17">
-        <v>0.13881196800000001</v>
+        <v>0.25839712300000001</v>
       </c>
       <c r="E17">
-        <v>8.8170603E-2</v>
+        <v>0.20636629400000001</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -9248,16 +9243,16 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>0.283129083</v>
+        <v>0.24763236499999999</v>
       </c>
       <c r="C18">
-        <v>0.20046145500000001</v>
+        <v>0.28567655600000003</v>
       </c>
       <c r="D18">
-        <v>0.13881196600000001</v>
+        <v>0.25839699300000002</v>
       </c>
       <c r="E18">
-        <v>8.8166570999999999E-2</v>
+        <v>0.20636626899999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -9265,16 +9260,16 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>0.28312975099999999</v>
+        <v>0.247215037</v>
       </c>
       <c r="C19">
-        <v>0.20046145500000001</v>
+        <v>0.28567296199999997</v>
       </c>
       <c r="D19">
-        <v>0.13881196500000001</v>
+        <v>0.25839693899999999</v>
       </c>
       <c r="E19">
-        <v>8.8163399000000003E-2</v>
+        <v>0.206366259</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -9282,16 +9277,16 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>0.28312975099999999</v>
+        <v>0.24690520699999999</v>
       </c>
       <c r="C20">
-        <v>0.20046145500000001</v>
+        <v>0.28567097200000002</v>
       </c>
       <c r="D20">
-        <v>0.13881262999999999</v>
+        <v>0.258396917</v>
       </c>
       <c r="E20">
-        <v>8.8161404999999998E-2</v>
+        <v>0.206366254</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -9299,16 +9294,16 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>0.28312975099999999</v>
+        <v>0.24667425600000001</v>
       </c>
       <c r="C21">
-        <v>0.20046145500000001</v>
+        <v>0.28566986100000002</v>
       </c>
       <c r="D21">
-        <v>0.13881262999999999</v>
+        <v>0.25839690700000001</v>
       </c>
       <c r="E21">
-        <v>8.8160349999999998E-2</v>
+        <v>0.206366253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add arbitry time check, add more graphics
</commit_message>
<xml_diff>
--- a/Excel_Data/2.xlsx
+++ b/Excel_Data/2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18324" windowHeight="9372" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18324" windowHeight="9372"/>
   </bookViews>
   <sheets>
     <sheet name="Лист5" sheetId="5" r:id="rId1"/>
@@ -805,11 +805,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-807433328"/>
-        <c:axId val="-807425168"/>
+        <c:axId val="683412256"/>
+        <c:axId val="989084288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-807433328"/>
+        <c:axId val="683412256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -852,7 +852,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-807425168"/>
+        <c:crossAx val="989084288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -860,7 +860,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-807425168"/>
+        <c:axId val="989084288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -911,7 +911,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-807433328"/>
+        <c:crossAx val="683412256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1685,11 +1685,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-804421456"/>
-        <c:axId val="-804414384"/>
+        <c:axId val="989464720"/>
+        <c:axId val="989456016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-804421456"/>
+        <c:axId val="989464720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1732,7 +1732,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804414384"/>
+        <c:crossAx val="989456016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1740,7 +1740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-804414384"/>
+        <c:axId val="989456016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1791,7 +1791,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804421456"/>
+        <c:crossAx val="989464720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1805,7 +1805,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2289,11 +2288,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-815684864"/>
-        <c:axId val="-815687040"/>
+        <c:axId val="989082112"/>
+        <c:axId val="989081568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-815684864"/>
+        <c:axId val="989082112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2336,7 +2335,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815687040"/>
+        <c:crossAx val="989081568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2344,7 +2343,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-815687040"/>
+        <c:axId val="989081568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2395,7 +2394,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815684864"/>
+        <c:crossAx val="989082112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3169,11 +3168,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-815688128"/>
-        <c:axId val="-815680512"/>
+        <c:axId val="989083744"/>
+        <c:axId val="989085376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-815688128"/>
+        <c:axId val="989083744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3216,7 +3215,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815680512"/>
+        <c:crossAx val="989085376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3224,7 +3223,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-815680512"/>
+        <c:axId val="989085376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3275,7 +3274,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815688128"/>
+        <c:crossAx val="989083744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4049,11 +4048,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-815676160"/>
-        <c:axId val="-815689216"/>
+        <c:axId val="989085920"/>
+        <c:axId val="989082656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-815676160"/>
+        <c:axId val="989085920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4096,7 +4095,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815689216"/>
+        <c:crossAx val="989082656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4104,7 +4103,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-815689216"/>
+        <c:axId val="989082656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4155,7 +4154,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815676160"/>
+        <c:crossAx val="989085920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4929,11 +4928,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-815686496"/>
-        <c:axId val="-815678880"/>
+        <c:axId val="989452752"/>
+        <c:axId val="989454928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-815686496"/>
+        <c:axId val="989452752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4976,7 +4975,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815678880"/>
+        <c:crossAx val="989454928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4984,7 +4983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-815678880"/>
+        <c:axId val="989454928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5035,7 +5034,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-815686496"/>
+        <c:crossAx val="989452752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5840,11 +5839,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-807432240"/>
-        <c:axId val="-807424080"/>
+        <c:axId val="989459280"/>
+        <c:axId val="989457104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-807432240"/>
+        <c:axId val="989459280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5887,7 +5886,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-807424080"/>
+        <c:crossAx val="989457104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5895,7 +5894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-807424080"/>
+        <c:axId val="989457104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5946,7 +5945,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-807432240"/>
+        <c:crossAx val="989459280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6720,11 +6719,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1119218208"/>
-        <c:axId val="-1119223104"/>
+        <c:axId val="989461456"/>
+        <c:axId val="989458192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1119218208"/>
+        <c:axId val="989461456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6767,7 +6766,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119223104"/>
+        <c:crossAx val="989458192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6775,7 +6774,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1119223104"/>
+        <c:axId val="989458192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6826,7 +6825,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1119218208"/>
+        <c:crossAx val="989461456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6840,7 +6839,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6922,7 +6920,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7631,11 +7628,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-804411664"/>
-        <c:axId val="-804412752"/>
+        <c:axId val="989460912"/>
+        <c:axId val="989454384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-804411664"/>
+        <c:axId val="989460912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7678,7 +7675,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804412752"/>
+        <c:crossAx val="989454384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7686,7 +7683,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-804412752"/>
+        <c:axId val="989454384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7737,7 +7734,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804411664"/>
+        <c:crossAx val="989460912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7751,7 +7748,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8511,11 +8507,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-804424176"/>
-        <c:axId val="-804424720"/>
+        <c:axId val="989467440"/>
+        <c:axId val="989464176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-804424176"/>
+        <c:axId val="989467440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8558,7 +8554,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804424720"/>
+        <c:crossAx val="989464176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8566,7 +8562,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-804424720"/>
+        <c:axId val="989464176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8617,7 +8613,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-804424176"/>
+        <c:crossAx val="989467440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8631,7 +8627,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14873,7 +14868,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:E21"/>
     </sheetView>
   </sheetViews>
@@ -15246,7 +15241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>

</xml_diff>